<commit_message>
added support for JS evaluated showif, closes #8, #4
</commit_message>
<xml_diff>
--- a/documentation/Example files/all_widgets_with_values.xlsx
+++ b/documentation/Example files/all_widgets_with_values.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="190">
   <si>
     <t>mc</t>
   </si>
@@ -633,6 +633,12 @@
   </si>
   <si>
     <t>"jura"</t>
+  </si>
+  <si>
+    <t>mc_religion == 1</t>
+  </si>
+  <si>
+    <t>abode %contains% 'berlin'</t>
   </si>
 </sst>
 </file>
@@ -716,8 +722,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -753,13 +761,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1093,7 +1103,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1260,7 +1270,9 @@
       <c r="D8" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F8" s="8" t="s">
         <v>30</v>
       </c>
@@ -1284,7 +1296,9 @@
       <c r="D9" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F9" s="8" t="s">
         <v>43</v>
       </c>
@@ -1302,7 +1316,9 @@
       <c r="D10" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F10" s="8" t="s">
         <v>30</v>
       </c>
@@ -1326,7 +1342,9 @@
       <c r="D11" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F11" s="8" t="s">
         <v>30</v>
       </c>
@@ -1344,7 +1362,9 @@
       <c r="D12" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G12" s="8" t="s">
         <v>108</v>
       </c>
@@ -1368,7 +1388,9 @@
       <c r="D14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G14" s="8" t="s">
         <v>158</v>
       </c>
@@ -1382,7 +1404,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30">
+    <row r="15" spans="1:13" ht="45">
       <c r="B15" s="8" t="s">
         <v>39</v>
       </c>
@@ -1392,7 +1414,9 @@
       <c r="D15" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="G15" s="8" t="s">
         <v>109</v>
       </c>
@@ -1416,7 +1440,9 @@
       <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G16" s="8" t="s">
         <v>159</v>
       </c>
@@ -1437,7 +1463,9 @@
       <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G17" s="8" t="s">
         <v>117</v>
       </c>
@@ -1452,7 +1480,9 @@
       <c r="D18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G18" s="8" t="s">
         <v>149</v>
       </c>
@@ -1469,11 +1499,13 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="30">
       <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M19" s="9" t="s">
         <v>185</v>
       </c>
@@ -1485,7 +1517,9 @@
       <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G20" s="8" t="s">
         <v>118</v>
       </c>
@@ -1500,7 +1534,9 @@
       <c r="D21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G21" s="8" t="s">
         <v>170</v>
       </c>
@@ -1521,7 +1557,9 @@
       <c r="D22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G22" s="8" t="s">
         <v>166</v>
       </c>
@@ -1542,7 +1580,9 @@
       <c r="D23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G23" s="8" t="s">
         <v>135</v>
       </c>
@@ -1550,24 +1590,30 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="E24" s="3"/>
+    <row r="24" spans="1:13" ht="30">
+      <c r="E24" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M24" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
-      <c r="E25" s="3"/>
+    <row r="25" spans="1:13" ht="30">
+      <c r="E25" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M25" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="33">
+    <row r="26" spans="1:13" ht="34">
       <c r="A26" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M26" s="9" t="s">
         <v>185</v>
       </c>
@@ -1579,7 +1625,9 @@
       <c r="D27" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G27" s="8" t="s">
         <v>121</v>
       </c>
@@ -1594,7 +1642,9 @@
       <c r="D28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G28" s="8" t="s">
         <v>122</v>
       </c>
@@ -1715,7 +1765,9 @@
       <c r="D37" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G37" s="8" t="s">
         <v>167</v>
       </c>
@@ -1730,7 +1782,9 @@
       <c r="D38" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G38" s="8" t="s">
         <v>168</v>
       </c>
@@ -1755,14 +1809,16 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" ht="30">
       <c r="C40" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G40" s="8" t="s">
         <v>59</v>
       </c>
@@ -1770,8 +1826,10 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
-      <c r="E41" s="3"/>
+    <row r="41" spans="1:13" ht="30">
+      <c r="E41" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M41" s="9" t="s">
         <v>185</v>
       </c>
@@ -1783,7 +1841,9 @@
       <c r="D42" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G42" s="8" t="s">
         <v>161</v>
       </c>
@@ -1798,7 +1858,9 @@
       <c r="D43" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G43" s="8" t="s">
         <v>124</v>
       </c>
@@ -1806,14 +1868,16 @@
         <v>185</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" ht="30">
       <c r="C44" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G44" s="8" t="s">
         <v>65</v>
       </c>
@@ -1828,7 +1892,9 @@
       <c r="D45" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G45" s="8" t="s">
         <v>125</v>
       </c>
@@ -1836,8 +1902,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
-      <c r="E46" s="3"/>
+    <row r="46" spans="1:13" ht="30">
+      <c r="E46" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M46" s="9" t="s">
         <v>185</v>
       </c>
@@ -1849,7 +1917,9 @@
       <c r="D47" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G47" s="8" t="s">
         <v>172</v>
       </c>
@@ -1867,7 +1937,9 @@
       <c r="D48" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="G48" s="8" t="s">
         <v>171</v>
       </c>
@@ -1878,20 +1950,26 @@
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="2:13">
-      <c r="E49" s="3"/>
+    <row r="49" spans="2:13" ht="30">
+      <c r="E49" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M49" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="2:13">
-      <c r="E50" s="3"/>
+    <row r="50" spans="2:13" ht="30">
+      <c r="E50" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M50" s="9" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="2:13">
-      <c r="E51" s="3"/>
+    <row r="51" spans="2:13" ht="30">
+      <c r="E51" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="M51" s="9" t="s">
         <v>185</v>
       </c>
@@ -1904,7 +1982,9 @@
       <c r="D52" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="4" t="s">
         <v>126</v>
@@ -1928,7 +2008,9 @@
       <c r="D53" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
         <v>175</v>
@@ -1962,7 +2044,9 @@
       <c r="D54" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
         <v>127</v>
@@ -1996,7 +2080,9 @@
       <c r="D55" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
docs and test tables
</commit_message>
<xml_diff>
--- a/documentation/Example files/all_widgets_with_values.xlsx
+++ b/documentation/Example files/all_widgets_with_values.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="208">
   <si>
     <t>mc</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>range 1,100,1</t>
-  </si>
-  <si>
-    <t>(Zeilen ohne Variablenname werden ignoriert und können zur Strukturierung benutzt werden.)</t>
   </si>
   <si>
     <t>slider_list</t>
@@ -340,10 +337,6 @@
   <si>
     <t>## TEXT
 Where do you live?</t>
-  </si>
-  <si>
-    <t>### MC
-&lt;sup title="If you can't make up your mind, you probably want to click Cthulhu." class="hastooltip"&gt;&lt;i class="icon-circle-blank"&gt;&lt;/i&gt;&lt;/sup&gt;  A simple multiple-choice question with two choices (and a hint).</t>
   </si>
   <si>
     <t>### MC
@@ -629,9 +622,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>#FF00FF</t>
-  </si>
-  <si>
     <t>"jura"</t>
   </si>
   <si>
@@ -639,6 +629,71 @@
   </si>
   <si>
     <t>abode %contains% 'berlin'</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>"Say what?"</t>
+  </si>
+  <si>
+    <t>"Berlin"</t>
+  </si>
+  <si>
+    <t>### MC
+&lt;sup title="If you can't make up your mind, you probably want to click Cthulhu." class="hastooltip"&gt;&lt;i class="icon-circle-blank"&gt;&lt;/i&gt;&lt;/sup&gt;  A simple multiple-choice question with two choices (and a hint).
+Click Cthulhu to show the other items!</t>
+  </si>
+  <si>
+    <t>bla@example.com</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>(Rows without a variable name are ignored and can be used for structure.)</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>11:01</t>
+  </si>
+  <si>
+    <t>29.04.1989</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>911</t>
+  </si>
+  <si>
+    <t>http://formr.org</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>#ff00ff</t>
+  </si>
+  <si>
+    <t>mc_button1</t>
+  </si>
+  <si>
+    <t>mc_button2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>mc-width70</t>
+  </si>
+  <si>
+    <t>"The Wire"</t>
   </si>
 </sst>
 </file>
@@ -722,7 +777,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -732,8 +787,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -760,16 +820,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1102,8 +1168,8 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1122,73 +1188,67 @@
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="18">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="225">
       <c r="C2" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45">
       <c r="C3" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E3" s="3"/>
       <c r="G3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1196,44 +1256,41 @@
         <v>7</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="M4" s="9" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="5" spans="1:13" ht="30">
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>185</v>
+        <v>103</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30">
       <c r="B6" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="3"/>
       <c r="G6" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="90">
+        <v>100</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="105">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1241,11 +1298,11 @@
         <v>0</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="8" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>20</v>
@@ -1254,7 +1311,7 @@
         <v>21</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="90">
@@ -1262,25 +1319,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="105">
@@ -1288,51 +1345,51 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="M9" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60">
       <c r="C10" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="75">
@@ -1340,19 +1397,19 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>185</v>
+        <v>105</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="180">
@@ -1360,74 +1417,71 @@
         <v>34</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="E13" s="3"/>
-      <c r="M13" s="9" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="14" spans="1:13" ht="135">
       <c r="B14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="45">
       <c r="B15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30">
@@ -1441,50 +1495,50 @@
         <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="30">
       <c r="C17" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="45">
       <c r="C18" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>13</v>
@@ -1496,17 +1550,14 @@
         <v>15</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30">
       <c r="A19" s="10" t="s">
-        <v>36</v>
+        <v>193</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M19" s="9" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1518,59 +1569,59 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30">
       <c r="C21" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30">
       <c r="C22" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45">
@@ -1581,29 +1632,29 @@
         <v>26</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30">
       <c r="E24" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30">
       <c r="E25" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="34">
@@ -1612,51 +1663,48 @@
       </c>
       <c r="B26" s="12"/>
       <c r="E26" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="30">
       <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45">
       <c r="C28" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="E29" s="3"/>
-      <c r="M29" s="9" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="30" spans="1:13" ht="30">
       <c r="C30" s="8" t="s">
@@ -1666,328 +1714,319 @@
         <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="C31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="M31" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="C32" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="C33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="C34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="M34" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="E35" s="3"/>
       <c r="M35" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="45">
       <c r="A36" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E36" s="3"/>
       <c r="M36" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="75">
       <c r="C37" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="E37" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30">
       <c r="C38" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>185</v>
+        <v>166</v>
+      </c>
+      <c r="M38" s="14" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="C39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="E39" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30">
       <c r="C40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="M40" s="9" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="30">
       <c r="E41" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="45">
       <c r="C42" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30">
       <c r="C43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>62</v>
-      </c>
       <c r="E43" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M43" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="30">
       <c r="C44" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G44" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="M44" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="45">
       <c r="C45" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30">
       <c r="E46" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="45">
       <c r="C47" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D47" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H47" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="M47" s="9" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="45">
       <c r="C48" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="2:13" ht="30">
       <c r="E49" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M49" s="9" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="50" spans="2:13" ht="30">
       <c r="E50" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M50" s="9" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="51" spans="2:13" ht="30">
       <c r="E51" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="M51" s="9" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="52" spans="2:13" ht="30">
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -1995,122 +2034,188 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="2:13" ht="60">
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H53" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J53" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="K53" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J53" s="3" t="s">
+      <c r="L53" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K53" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="M53" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="2:13" ht="45">
       <c r="B54" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H54" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="I54" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J54" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="K54" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J54" s="3" t="s">
+      <c r="L54" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="M54" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="2:13" ht="45">
       <c r="B55" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="J55" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="K55" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="L55" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K55" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="M55" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13">
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="2:13">
-      <c r="E57" s="3"/>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" ht="30">
+      <c r="B56" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M56" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" ht="30">
+      <c r="B57" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="M57" s="9" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="58" spans="2:13">
       <c r="C58" s="8" t="s">
@@ -2121,31 +2226,35 @@
       </c>
       <c r="E58" s="3"/>
       <c r="G58" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M58" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="2:13" ht="195">
       <c r="C59" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M59" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="G42:G45"/>
+  <hyperlinks>
+    <hyperlink ref="M11" r:id="rId1"/>
+    <hyperlink ref="M38" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -2172,19 +2281,19 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2235,21 +2344,21 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>